<commit_message>
MSA median salesprice update
</commit_message>
<xml_diff>
--- a/MSA_Med Sale Price.xlsx
+++ b/MSA_Med Sale Price.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kayla\Documents\GitHub\QuantitativeAssignment1_KM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2955631B-7994-4AD7-94DA-69A8BB1168E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDD04C6-1E4B-4A83-A494-E54AB36D8506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1700" yWindow="1700" windowWidth="2370" windowHeight="560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MSA For Sale Inventory" sheetId="1" r:id="rId1"/>
@@ -456,31 +456,31 @@
     <t>Fort Collins, CO</t>
   </si>
   <si>
-    <t>Inv_Jan</t>
-  </si>
-  <si>
-    <t>Inv_Feb</t>
-  </si>
-  <si>
-    <t>Inv_Mar</t>
-  </si>
-  <si>
-    <t>Inv_Apr</t>
-  </si>
-  <si>
-    <t>Inv_May</t>
-  </si>
-  <si>
-    <t>Inv_June</t>
-  </si>
-  <si>
-    <t>Inv_Jul</t>
-  </si>
-  <si>
-    <t>Inv_Aug</t>
-  </si>
-  <si>
-    <t>Inv_Sep</t>
+    <t>SaleP_Jan</t>
+  </si>
+  <si>
+    <t>SaleP_Feb</t>
+  </si>
+  <si>
+    <t>SaleP_Mar</t>
+  </si>
+  <si>
+    <t>SaleP_Apr</t>
+  </si>
+  <si>
+    <t>SaleP_May</t>
+  </si>
+  <si>
+    <t>SaleP_June</t>
+  </si>
+  <si>
+    <t>SaleP_Jul</t>
+  </si>
+  <si>
+    <t>SaleP_Aug</t>
+  </si>
+  <si>
+    <t>SaleP_Sep</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1325,7 @@
   <dimension ref="A1:N96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>